<commit_message>
fixed bugs, added crvPay
</commit_message>
<xml_diff>
--- a/generated.xlsx
+++ b/generated.xlsx
@@ -385,19 +385,20 @@
       <c r="A1" t="str">
         <v>ግብር ከፋይ መለያ ቁጥር - 0062451276</v>
       </c>
-      <c r="B1" t="str">
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
         <v>የግብር ከፋይ ስም - El-Hadar Engineering &amp; Trading P.L.C</v>
       </c>
-      <c r="C1" t="str">
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>የስራው ዓይነት - Almunium &amp; Metal &amp; Electro Mechanical Work</v>
-      </c>
-      <c r="D1" t="str">
-        <v>ሪፖርት የተደረገበት ወር - Sat Dec 12 2020 - Up To : Tue Dec 12 2023</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v/>
+        <v>ሪፖርት የተደረገበት ወር - Sat Dec 12 2020 - Up To : Tue Dec 12 2023</v>
       </c>
       <c r="B4" t="str">
         <v/>
@@ -407,6 +408,18 @@
       </c>
       <c r="D4" t="str">
         <v>የተከፈለው ገንዘብ መጠን በብር</v>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v>ግዢው የተፈፀመበት ደረሰኝ</v>
       </c>
     </row>
     <row r="5">
@@ -440,10 +453,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>0</v>
+        <v>01</v>
       </c>
       <c r="B6" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C6" t="str">
         <v>100</v>
@@ -469,10 +482,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B7" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C7" t="str">
         <v>100</v>
@@ -498,10 +511,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B8" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C8" t="str">
         <v>100</v>
@@ -527,10 +540,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B9" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C9" t="str">
         <v>100</v>
@@ -556,10 +569,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B10" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C10" t="str">
         <v>100</v>
@@ -585,10 +598,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B11" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C11" t="str">
         <v>100</v>
@@ -614,10 +627,10 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B12" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C12" t="str">
         <v>100</v>
@@ -643,10 +656,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B13" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C13" t="str">
         <v>100</v>
@@ -672,10 +685,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B14" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C14" t="str">
         <v>100</v>
@@ -701,10 +714,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="B15" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C15" t="str">
         <v>100</v>
@@ -730,10 +743,10 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="B16" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C16" t="str">
         <v>100</v>
@@ -759,10 +772,10 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B17" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C17" t="str">
         <v>100</v>
@@ -788,10 +801,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B18" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C18" t="str">
         <v>100</v>
@@ -817,10 +830,10 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="B19" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C19" t="str">
         <v>100</v>
@@ -846,10 +859,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="B20" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C20" t="str">
         <v>100</v>
@@ -875,10 +888,10 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="B21" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C21" t="str">
         <v>100</v>
@@ -904,10 +917,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="B22" t="str">
-        <v>Hello</v>
+        <v>[object Object]</v>
       </c>
       <c r="C22" t="str">
         <v>100</v>

</xml_diff>